<commit_message>
streamlit app framed with working metrics and map
</commit_message>
<xml_diff>
--- a/data/apra-2014-2021.xlsx
+++ b/data/apra-2014-2021.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anthonytownsend/Dropbox/Desktop/_CODE/notebooks/jc_APRA/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anthonytownsend/Dropbox/Desktop/_code/notebooks/jc_APRA/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87BA1092-E9B4-0642-9D1A-D434B113FE3F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2967A41-F303-DE4A-BF84-89F49895EA37}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="68800" windowHeight="28300" xr2:uid="{0A09606D-EC16-2A43-84C6-614E2A34B3ED}"/>
   </bookViews>
@@ -1106,8 +1106,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B49183E2-ADCB-4043-8D4F-D33B19FD53EE}">
   <dimension ref="A1:O180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
-      <selection activeCell="F98" sqref="F98"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48:B73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2240,7 +2240,7 @@
         <v>128</v>
       </c>
       <c r="B48" s="7">
-        <v>42917</v>
+        <v>42736</v>
       </c>
       <c r="C48" s="3" t="s">
         <v>165</v>
@@ -2265,7 +2265,7 @@
         <v>128</v>
       </c>
       <c r="B49" s="7">
-        <v>42917</v>
+        <v>42736</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>166</v>
@@ -2290,7 +2290,7 @@
         <v>128</v>
       </c>
       <c r="B50" s="7">
-        <v>42917</v>
+        <v>42736</v>
       </c>
       <c r="C50" s="3" t="s">
         <v>167</v>
@@ -2315,7 +2315,7 @@
         <v>128</v>
       </c>
       <c r="B51" s="7">
-        <v>42917</v>
+        <v>42736</v>
       </c>
       <c r="C51" s="3" t="s">
         <v>168</v>
@@ -2340,7 +2340,7 @@
         <v>128</v>
       </c>
       <c r="B52" s="7">
-        <v>42917</v>
+        <v>42736</v>
       </c>
       <c r="C52" s="3" t="s">
         <v>170</v>
@@ -2365,7 +2365,7 @@
         <v>128</v>
       </c>
       <c r="B53" s="7">
-        <v>42917</v>
+        <v>42736</v>
       </c>
       <c r="C53" s="3" t="s">
         <v>171</v>
@@ -2390,7 +2390,7 @@
         <v>128</v>
       </c>
       <c r="B54" s="7">
-        <v>42917</v>
+        <v>42736</v>
       </c>
       <c r="C54" s="3" t="s">
         <v>172</v>
@@ -2415,7 +2415,7 @@
         <v>128</v>
       </c>
       <c r="B55" s="7">
-        <v>42917</v>
+        <v>42736</v>
       </c>
       <c r="C55" s="3" t="s">
         <v>174</v>
@@ -2440,7 +2440,7 @@
         <v>128</v>
       </c>
       <c r="B56" s="7">
-        <v>42917</v>
+        <v>42736</v>
       </c>
       <c r="C56" s="3" t="s">
         <v>175</v>
@@ -2465,7 +2465,7 @@
         <v>128</v>
       </c>
       <c r="B57" s="7">
-        <v>42917</v>
+        <v>42736</v>
       </c>
       <c r="C57" s="3" t="s">
         <v>176</v>
@@ -2490,7 +2490,7 @@
         <v>128</v>
       </c>
       <c r="B58" s="7">
-        <v>42917</v>
+        <v>42736</v>
       </c>
       <c r="C58" s="3" t="s">
         <v>34</v>
@@ -2515,7 +2515,7 @@
         <v>128</v>
       </c>
       <c r="B59" s="7">
-        <v>42917</v>
+        <v>42736</v>
       </c>
       <c r="C59" s="3" t="s">
         <v>177</v>
@@ -2540,7 +2540,7 @@
         <v>128</v>
       </c>
       <c r="B60" s="7">
-        <v>42917</v>
+        <v>42736</v>
       </c>
       <c r="C60" s="3" t="s">
         <v>221</v>
@@ -2565,7 +2565,7 @@
         <v>128</v>
       </c>
       <c r="B61" s="7">
-        <v>42917</v>
+        <v>42736</v>
       </c>
       <c r="C61" s="3" t="s">
         <v>178</v>
@@ -2590,7 +2590,7 @@
         <v>128</v>
       </c>
       <c r="B62" s="7">
-        <v>42917</v>
+        <v>42736</v>
       </c>
       <c r="C62" s="3" t="s">
         <v>179</v>
@@ -2615,7 +2615,7 @@
         <v>128</v>
       </c>
       <c r="B63" s="7">
-        <v>42917</v>
+        <v>42736</v>
       </c>
       <c r="C63" s="3" t="s">
         <v>186</v>
@@ -2640,7 +2640,7 @@
         <v>128</v>
       </c>
       <c r="B64" s="7">
-        <v>42917</v>
+        <v>42736</v>
       </c>
       <c r="C64" s="3" t="s">
         <v>187</v>
@@ -2665,7 +2665,7 @@
         <v>128</v>
       </c>
       <c r="B65" s="7">
-        <v>42917</v>
+        <v>42736</v>
       </c>
       <c r="C65" s="3" t="s">
         <v>188</v>
@@ -2690,7 +2690,7 @@
         <v>128</v>
       </c>
       <c r="B66" s="7">
-        <v>42917</v>
+        <v>42736</v>
       </c>
       <c r="C66" s="3" t="s">
         <v>189</v>
@@ -2715,7 +2715,7 @@
         <v>128</v>
       </c>
       <c r="B67" s="7">
-        <v>42917</v>
+        <v>42736</v>
       </c>
       <c r="C67" s="3" t="s">
         <v>184</v>
@@ -2740,7 +2740,7 @@
         <v>128</v>
       </c>
       <c r="B68" s="7">
-        <v>42917</v>
+        <v>42736</v>
       </c>
       <c r="C68" s="3" t="s">
         <v>190</v>
@@ -2765,7 +2765,7 @@
         <v>128</v>
       </c>
       <c r="B69" s="7">
-        <v>42917</v>
+        <v>42736</v>
       </c>
       <c r="C69" s="3" t="s">
         <v>191</v>
@@ -2790,7 +2790,7 @@
         <v>128</v>
       </c>
       <c r="B70" s="7">
-        <v>42917</v>
+        <v>42736</v>
       </c>
       <c r="C70" s="3" t="s">
         <v>192</v>
@@ -2815,7 +2815,7 @@
         <v>128</v>
       </c>
       <c r="B71" s="7">
-        <v>42917</v>
+        <v>42736</v>
       </c>
       <c r="C71" s="3" t="s">
         <v>193</v>
@@ -2840,7 +2840,7 @@
         <v>128</v>
       </c>
       <c r="B72" s="7">
-        <v>42917</v>
+        <v>42736</v>
       </c>
       <c r="C72" s="3" t="s">
         <v>194</v>
@@ -2865,7 +2865,7 @@
         <v>128</v>
       </c>
       <c r="B73" s="7">
-        <v>42917</v>
+        <v>42736</v>
       </c>
       <c r="C73" s="3" t="s">
         <v>195</v>

</xml_diff>